<commit_message>
adit Skill data table
add category
</commit_message>
<xml_diff>
--- a/Assets/ExcelDataTables/SkillData.xlsx
+++ b/Assets/ExcelDataTables/SkillData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SSH\Desktop\Unity Project\UnityKoreaAward\Assets\ExcelDataTables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UnityProject\UnityKoreaAward\Assets\ExcelDataTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A5D032-224B-4D26-9C8B-477D03515ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC80F64-36AC-4E58-A4C6-61A20BFA791A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8604FDB5-84BE-4B51-A6B9-BF38D8CD2456}"/>
+    <workbookView xWindow="1590" yWindow="1470" windowWidth="26505" windowHeight="13515" xr2:uid="{8604FDB5-84BE-4B51-A6B9-BF38D8CD2456}"/>
   </bookViews>
   <sheets>
     <sheet name="ActiveSkilll" sheetId="1" r:id="rId1"/>
@@ -297,7 +297,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{9AC6471B-FA77-4F63-B493-BBD77DCA4BD7}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{9AC6471B-FA77-4F63-B493-BBD77DCA4BD7}">
       <text>
         <r>
           <rPr>
@@ -419,7 +419,256 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{174D498E-EAA4-4A23-95F1-72C5EA92DE9C}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{62C5B0CE-9D62-47D8-B33A-8C9B37D45F02}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>신성환</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>든화율</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{DEF30E4E-0190-47D1-AA7D-E0742104C5BA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>신성환</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>피격</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>시</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>효과</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>범위</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{C5FF459E-1FC4-4041-984F-43500AC8951E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>신성환</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>관통</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>가능한</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>유닛</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>수</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{174D498E-EAA4-4A23-95F1-72C5EA92DE9C}">
       <text>
         <r>
           <rPr>
@@ -1342,7 +1591,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>Id::int</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1371,10 +1620,6 @@
     <t>DoubleShot</t>
   </si>
   <si>
-    <t>총알을 2발 발사</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MultiShot</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1471,6 +1716,59 @@
   </si>
   <si>
     <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Skill Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ranged Skill
+(원거리 스킬)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Melee Skill
+(근접 스킬)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Installation Skill
+(설치형 스킬)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Drone Skill
+(드론 스킬)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EffectRange::float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NumberOfBullets</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SlowdownRate::float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NumberOfPenetratingUnit::int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaxLevel::int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본 효과 : 직선 방향으로 총알을 2발 발사
+레벨업 효과 : 쿨타임 -0.5 / 스킬 데미지 + 0.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Depth::int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1551,7 +1849,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1560,6 +1858,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1597,25 +1907,21 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BC7EB365-364F-4604-B79F-71F633412323}" name="표3" displayName="표3" ref="I1:I1000" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="I1:I1000" xr:uid="{BC7EB365-364F-4604-B79F-71F633412323}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BC7EB365-364F-4604-B79F-71F633412323}" name="표3" displayName="표3" ref="P1:P1019" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="P1:P1019" xr:uid="{BC7EB365-364F-4604-B79F-71F633412323}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B052816E-B949-49E7-8682-F13E79AA6940}" name="PlayerSkillType DropBox List" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{B052816E-B949-49E7-8682-F13E79AA6940}" name="PlayerSkillType DropBox List" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8391DFAE-F7CD-42C5-8228-62914558822A}" name="표3_5" displayName="표3_5" ref="L1:L1001" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8391DFAE-F7CD-42C5-8228-62914558822A}" name="표3_5" displayName="표3_5" ref="L1:L1001" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
   <autoFilter ref="L1:L1001" xr:uid="{8391DFAE-F7CD-42C5-8228-62914558822A}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{028EE81F-3896-4DD1-8E4E-D34976DDD1EE}" name="PlayerSkillType DropBox List" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{028EE81F-3896-4DD1-8E4E-D34976DDD1EE}" name="PlayerSkillType DropBox List" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1918,27 +2224,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D55F758D-E215-4074-A7E1-6D216D7A2AF4}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.5" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="30.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="1"/>
+    <col min="5" max="5" width="12.25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.75" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="17.5" style="1" customWidth="1"/>
+    <col min="16" max="16" width="30.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1952,65 +2265,233 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O3" s="4"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O4" s="4"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O5" s="4"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O6" s="4"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O7" s="4"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O8" s="4"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O9" s="5"/>
+      <c r="P9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O10" s="5"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O11" s="5"/>
+      <c r="P11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="1">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I4" s="1" t="s">
-        <v>8</v>
-      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O12" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O13" s="4"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O14" s="4"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O15" s="4"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O16" s="4"/>
+    </row>
+    <row r="17" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O17" s="4"/>
+    </row>
+    <row r="18" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O18" s="4"/>
+    </row>
+    <row r="19" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O19" s="5"/>
+    </row>
+    <row r="20" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O20" s="5"/>
+    </row>
+    <row r="21" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O21" s="5"/>
+    </row>
+    <row r="22" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O22" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O23" s="4"/>
+    </row>
+    <row r="24" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O24" s="4"/>
+    </row>
+    <row r="25" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O25" s="4"/>
+    </row>
+    <row r="26" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O26" s="4"/>
+    </row>
+    <row r="27" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O27" s="4"/>
+    </row>
+    <row r="28" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O28" s="4"/>
+    </row>
+    <row r="29" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O29" s="4"/>
+    </row>
+    <row r="30" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O30" s="4"/>
+    </row>
+    <row r="31" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O31" s="4"/>
+    </row>
+    <row r="32" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O32" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O33" s="4"/>
+    </row>
+    <row r="34" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O34" s="4"/>
+    </row>
+    <row r="35" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O35" s="4"/>
+    </row>
+    <row r="36" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O36" s="4"/>
+    </row>
+    <row r="37" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O37" s="4"/>
+    </row>
+    <row r="38" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O38" s="4"/>
+    </row>
+    <row r="39" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O39" s="4"/>
+    </row>
+    <row r="40" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O40" s="4"/>
+    </row>
+    <row r="41" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O41" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="O2:O11"/>
+    <mergeCell ref="O12:O21"/>
+    <mergeCell ref="O22:O31"/>
+    <mergeCell ref="O32:O41"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{45CB9A8E-11F7-4871-9D44-19F2C3D7774B}">
-      <formula1>$I$2:$I$1000</formula1>
+      <formula1>$P$2:$P$1019</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2020,7 +2501,8 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2035,7 +2517,7 @@
     <col min="9" max="9" width="18.5" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.5" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" style="1"/>
-    <col min="12" max="12" width="11.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -2056,22 +2538,22 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -2079,13 +2561,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="1">
         <v>5</v>
@@ -2106,7 +2588,7 @@
         <v>5</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -2114,13 +2596,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1">
         <v>5</v>
@@ -2141,7 +2623,7 @@
         <v>5</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -2149,13 +2631,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="1">
         <v>5</v>
@@ -2176,7 +2658,7 @@
         <v>5</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -2184,13 +2666,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1">
         <v>5</v>
@@ -2211,7 +2693,7 @@
         <v>5</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -2219,13 +2701,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="1">
         <v>5</v>
@@ -2246,7 +2728,7 @@
         <v>0.5</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reset bullet sprite renderer
</commit_message>
<xml_diff>
--- a/Assets/ExcelDataTables/SkillData.xlsx
+++ b/Assets/ExcelDataTables/SkillData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SSH\Desktop\Unity Project\UnityKoreaAward\Assets\ExcelDataTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E699F46-F328-4E07-A1B2-230F5657B8D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263D4568-492A-4A4D-8B5B-4F744A256392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4350" yWindow="465" windowWidth="17340" windowHeight="13545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23175" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ActiveSkilll" sheetId="1" r:id="rId1"/>
@@ -2074,7 +2074,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="87">
   <si>
     <t>Fire Tower</t>
   </si>
@@ -2102,260 +2102,270 @@
     <t>Ultamate SafeZone</t>
   </si>
   <si>
+    <t>기본 효과 : 적중 시 광범위한 폭발 발생
+레벨업 효과 : 폭발 범위 증가 1.5(곱연산) / 스킬 데미지 +1 / 쿨타임 - 0.5</t>
+  </si>
+  <si>
+    <t>기본 효과 : 매 초 전체 체력 비례 데미지
+레벨업 효과 : 쿨타임 -0.5 / 초당 피해 10%</t>
+  </si>
+  <si>
+    <t>기본 효과 : 적중 시 일정 확률로 Player HP 회복
+레벨업 효과 : 회복 확률 증가 +1%</t>
+  </si>
+  <si>
+    <t>기본 효과 : 적을 둔화 시키는 총알 발사
+레벨업 효과 : 쿨타임 -0.5 / 스킬 데미지 + 1 / 둔화율 10%</t>
+  </si>
+  <si>
+    <t>기본 효과 : 적중 시 블랙홀 중앙으로 중력 작용
+레벨업 효과 : 블랙홀 범위 증가 1.5(곱연산) / 쿨타임 -0.5</t>
+  </si>
+  <si>
+    <t>기본 효과 : 적을 관통하는 총알 발사
+레벨업 효과 : 관통 가능한 적 +1</t>
+  </si>
+  <si>
+    <t>기본 효과 : 적의 방어력을 일정 % 무시하는 공격 (보스는 50% 효과만 적용)
+레벨업 효과 : 적의 방어력 10% 추가 무시</t>
+  </si>
+  <si>
+    <t>기본 효과 : 적중 시 퍼지는 총알 발사
+레벨업 효과 : 퍼지는 총알 +2 (총알 증가에 따른 각도 변경) / 스킬 데미지 +1</t>
+  </si>
+  <si>
+    <t>PlayerSkillType DropBox List</t>
+  </si>
+  <si>
+    <t>NumberOfPenetratingUnit::int</t>
+  </si>
+  <si>
+    <t>EffectRange::float</t>
+  </si>
+  <si>
+    <t>RateOfFire::float</t>
+  </si>
+  <si>
+    <t>Melee Skill
+(근접 스킬)</t>
+  </si>
+  <si>
+    <t>DecreaseRate::float</t>
+  </si>
+  <si>
+    <t>PoisonRate::float</t>
+  </si>
+  <si>
+    <t>Drone Skill
+(드론 스킬)</t>
+  </si>
+  <si>
+    <t>SlowdownRate::float</t>
+  </si>
+  <si>
+    <t>UnlockLevel::int</t>
+  </si>
+  <si>
+    <t>SkillDamage::float</t>
+  </si>
+  <si>
+    <t>AddDamage::float</t>
+  </si>
+  <si>
+    <t>IncreaseRate::float</t>
+  </si>
+  <si>
+    <t>ShootingRate::float</t>
+  </si>
+  <si>
+    <t>Description::string</t>
+  </si>
+  <si>
+    <t>Shock Wave</t>
+  </si>
+  <si>
+    <t>PiercingShot</t>
+  </si>
+  <si>
+    <t>CoolTime::float</t>
+  </si>
+  <si>
+    <t>Name::string</t>
+  </si>
+  <si>
+    <t>MaxLevel::int</t>
+  </si>
+  <si>
+    <t>BlackHoleShot</t>
+  </si>
+  <si>
+    <t>Tower Explosion</t>
+  </si>
+  <si>
+    <t>Distributed Attack</t>
+  </si>
+  <si>
+    <t>공격력 증가</t>
+  </si>
+  <si>
+    <t>Id::int</t>
+  </si>
+  <si>
+    <t>연사력 증가</t>
+  </si>
+  <si>
+    <t>Defense</t>
+  </si>
+  <si>
+    <t>체력 증가</t>
+  </si>
+  <si>
+    <t>방어력 증가</t>
+  </si>
+  <si>
+    <t>마나 증가</t>
+  </si>
+  <si>
+    <t>RateOfFire</t>
+  </si>
+  <si>
+    <t>AddAttack</t>
+  </si>
+  <si>
+    <t>MultiShot</t>
+  </si>
+  <si>
+    <t>AddHp::int</t>
+  </si>
+  <si>
+    <t>HardShot</t>
+  </si>
+  <si>
+    <t>NerfShot</t>
+  </si>
+  <si>
+    <t>Skill Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DoubleShot </t>
+  </si>
+  <si>
+    <t>SlowingShot</t>
+  </si>
+  <si>
+    <t>RapidShot</t>
+  </si>
+  <si>
+    <t>AddMp::int</t>
+  </si>
+  <si>
+    <t>HealingShot</t>
+  </si>
+  <si>
+    <t>NapalmShot</t>
+  </si>
+  <si>
+    <t>PoisonShot</t>
+  </si>
+  <si>
+    <t>SplitShot</t>
+  </si>
+  <si>
+    <t>Ranged Skill
+(원거리 스킬)</t>
+  </si>
+  <si>
+    <t>PlayerSkiilsType::enum</t>
+  </si>
+  <si>
+    <t>NumberOfBullets::int</t>
+  </si>
+  <si>
+    <t>Installation Skill
+(설치형 스킬)</t>
+  </si>
+  <si>
+    <t>IgnoreDefenseRate::float</t>
+  </si>
+  <si>
+    <t>RateOfHealingShot::float</t>
+  </si>
+  <si>
+    <t>기본 효과 : 타워 주변에 플레이어의 HP를 회복시키는 영역을 생성
+레벨업 효과 : 지속 힐량 증가 / 범위 증가</t>
+  </si>
+  <si>
+    <t>기본 효과 : 적을 공격할때, 추가적인 총알들이 주변으로 퍼져 나감
+레벨업 효과 : 추가총알 개수와 범위 증가</t>
+  </si>
+  <si>
+    <t>기본 효과 : 설치된 타워들이 주변 적들에게 데미지를 주면 플레이어 체력 회복
+레벨업 효과 : 체력 회복량 증가</t>
+  </si>
+  <si>
+    <t>기본 효과 : 설치된 모든 타워들을 강화
+레벨업 효과 : float(++) 값을 통해 설치형 타워스킬들에 곱</t>
+  </si>
+  <si>
+    <t>기본 효과 : 일정 범위에 무적 존을 생성
+레벨업 효과 : 지속시간 증가 / 쿨타임 감소</t>
+  </si>
+  <si>
+    <t>기본 효과 : 맵 전체를 관통하는 충격파 생성(모든적 타격)
+레벨업 효과 : 데미지 증가</t>
+  </si>
+  <si>
+    <t>기본 효과 : 주변 적들에게 지속 데미지를 주는 타워
+레벨업 효과 : 지속 데미지 증가 / 범위 증가</t>
+  </si>
+  <si>
+    <t>기본 효과 : 주변 적들을 관통하는 레이저를 발사하는 타워
+레벨업 효과 : 관통 가능수와 데미지 증가</t>
+  </si>
+  <si>
+    <t>기본 효과 : 설치된 타워가 파괴될때 폭발하여 주변 적들에게 피해를줌
+레벨업 효과 : 데미지 / 범위 증가</t>
+  </si>
+  <si>
+    <t>기본 효과 : 필드내 무작위 지점에 독안개를 생성 (적이 밟으면 도트뎀)
+레벨업 효과 : 도트뎀 증가</t>
+  </si>
+  <si>
+    <t>Tower Reinforcement</t>
+  </si>
+  <si>
+    <t>HealingTower</t>
+  </si>
+  <si>
+    <t>VampireTower</t>
+  </si>
+  <si>
+    <t>PoisonTower</t>
+  </si>
+  <si>
+    <t>Depth::int</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Duration::float</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
     <t>기본 효과 : 몬스터의 기본 능력치 (공격력) 을 감소시킴 (보스는 50% 효과만 적용)
 레벨업 효과 : 능력치 감소율 10% 증가</t>
-  </si>
-  <si>
-    <t>기본 효과 : 적중 시 광범위한 폭발 발생
-레벨업 효과 : 폭발 범위 증가 1.5(곱연산) / 스킬 데미지 +1 / 쿨타임 - 0.5</t>
-  </si>
-  <si>
-    <t>기본 효과 : 매 초 전체 체력 비례 데미지
-레벨업 효과 : 쿨타임 -0.5 / 초당 피해 10%</t>
-  </si>
-  <si>
-    <t>기본 효과 : 적중 시 일정 확률로 Player HP 회복
-레벨업 효과 : 회복 확률 증가 +1%</t>
-  </si>
-  <si>
-    <t>기본 효과 : 적을 둔화 시키는 총알 발사
-레벨업 효과 : 쿨타임 -0.5 / 스킬 데미지 + 1 / 둔화율 10%</t>
-  </si>
-  <si>
-    <t>기본 효과 : 적중 시 블랙홀 중앙으로 중력 작용
-레벨업 효과 : 블랙홀 범위 증가 1.5(곱연산) / 쿨타임 -0.5</t>
-  </si>
-  <si>
-    <t>기본 효과 : 적을 관통하는 총알 발사
-레벨업 효과 : 관통 가능한 적 +1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>NerfShot</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>기본 효과 : 총알의 이동 속도와 연사 속도 상승
 레벨업 효과 : 총알의 이동속도 20%, 연사력 20% 상승</t>
-  </si>
-  <si>
-    <t>기본 효과 : 적의 방어력을 일정 % 무시하는 공격 (보스는 50% 효과만 적용)
-레벨업 효과 : 적의 방어력 10% 추가 무시</t>
-  </si>
-  <si>
-    <t>기본 효과 : 적중 시 퍼지는 총알 발사
-레벨업 효과 : 퍼지는 총알 +2 (총알 증가에 따른 각도 변경) / 스킬 데미지 +1</t>
-  </si>
-  <si>
-    <t>PlayerSkillType DropBox List</t>
-  </si>
-  <si>
-    <t>NumberOfPenetratingUnit::int</t>
-  </si>
-  <si>
-    <t>EffectRange::float</t>
-  </si>
-  <si>
-    <t>RateOfFire::float</t>
-  </si>
-  <si>
-    <t>Melee Skill
-(근접 스킬)</t>
-  </si>
-  <si>
-    <t>DecreaseRate::float</t>
-  </si>
-  <si>
-    <t>PoisonRate::float</t>
-  </si>
-  <si>
-    <t>Drone Skill
-(드론 스킬)</t>
-  </si>
-  <si>
-    <t>SlowdownRate::float</t>
-  </si>
-  <si>
-    <t>UnlockLevel::int</t>
-  </si>
-  <si>
-    <t>SkillDamage::float</t>
-  </si>
-  <si>
-    <t>AddDamage::float</t>
-  </si>
-  <si>
-    <t>IncreaseRate::float</t>
-  </si>
-  <si>
-    <t>ShootingRate::float</t>
-  </si>
-  <si>
-    <t>Description::string</t>
-  </si>
-  <si>
-    <t>Shock Wave</t>
-  </si>
-  <si>
-    <t>PiercingShot</t>
-  </si>
-  <si>
-    <t>CoolTime::float</t>
-  </si>
-  <si>
-    <t>Name::string</t>
-  </si>
-  <si>
-    <t>MaxLevel::int</t>
-  </si>
-  <si>
-    <t>BlackHoleShot</t>
-  </si>
-  <si>
-    <t>Tower Explosion</t>
-  </si>
-  <si>
-    <t>Distributed Attack</t>
-  </si>
-  <si>
-    <t>공격력 증가</t>
-  </si>
-  <si>
-    <t>Id::int</t>
-  </si>
-  <si>
-    <t>연사력 증가</t>
-  </si>
-  <si>
-    <t>Defense</t>
-  </si>
-  <si>
-    <t>체력 증가</t>
-  </si>
-  <si>
-    <t>방어력 증가</t>
-  </si>
-  <si>
-    <t>마나 증가</t>
-  </si>
-  <si>
-    <t>RateOfFire</t>
-  </si>
-  <si>
-    <t>AddAttack</t>
-  </si>
-  <si>
-    <t>MultiShot</t>
-  </si>
-  <si>
-    <t>AddHp::int</t>
-  </si>
-  <si>
-    <t>HardShot</t>
-  </si>
-  <si>
-    <t>NerfShot</t>
-  </si>
-  <si>
-    <t>Skill Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DoubleShot </t>
-  </si>
-  <si>
-    <t>SlowingShot</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>RapidShot</t>
-  </si>
-  <si>
-    <t>AddMp::int</t>
-  </si>
-  <si>
-    <t>HealingShot</t>
-  </si>
-  <si>
-    <t>NapalmShot</t>
-  </si>
-  <si>
-    <t>PoisonShot</t>
-  </si>
-  <si>
-    <t>SplitShot</t>
-  </si>
-  <si>
-    <t>Ranged Skill
-(원거리 스킬)</t>
-  </si>
-  <si>
-    <t>PlayerSkiilsType::enum</t>
-  </si>
-  <si>
-    <t>NumberOfBullets::int</t>
-  </si>
-  <si>
-    <t>Installation Skill
-(설치형 스킬)</t>
-  </si>
-  <si>
-    <t>IgnoreDefenseRate::float</t>
-  </si>
-  <si>
-    <t>RateOfHealingShot::float</t>
-  </si>
-  <si>
-    <t>기본 효과 : 타워 주변에 플레이어의 HP를 회복시키는 영역을 생성
-레벨업 효과 : 지속 힐량 증가 / 범위 증가</t>
-  </si>
-  <si>
-    <t>기본 효과 : 적을 공격할때, 추가적인 총알들이 주변으로 퍼져 나감
-레벨업 효과 : 추가총알 개수와 범위 증가</t>
-  </si>
-  <si>
-    <t>기본 효과 : 설치된 타워들이 주변 적들에게 데미지를 주면 플레이어 체력 회복
-레벨업 효과 : 체력 회복량 증가</t>
-  </si>
-  <si>
-    <t>기본 효과 : 설치된 모든 타워들을 강화
-레벨업 효과 : float(++) 값을 통해 설치형 타워스킬들에 곱</t>
-  </si>
-  <si>
-    <t>기본 효과 : 일정 범위에 무적 존을 생성
-레벨업 효과 : 지속시간 증가 / 쿨타임 감소</t>
-  </si>
-  <si>
-    <t>기본 효과 : 맵 전체를 관통하는 충격파 생성(모든적 타격)
-레벨업 효과 : 데미지 증가</t>
-  </si>
-  <si>
-    <t>기본 효과 : 주변 적들에게 지속 데미지를 주는 타워
-레벨업 효과 : 지속 데미지 증가 / 범위 증가</t>
-  </si>
-  <si>
-    <t>기본 효과 : 주변 적들을 관통하는 레이저를 발사하는 타워
-레벨업 효과 : 관통 가능수와 데미지 증가</t>
-  </si>
-  <si>
-    <t>기본 효과 : 설치된 타워가 파괴될때 폭발하여 주변 적들에게 피해를줌
-레벨업 효과 : 데미지 / 범위 증가</t>
-  </si>
-  <si>
-    <t>기본 효과 : 필드내 무작위 지점에 독안개를 생성 (적이 밟으면 도트뎀)
-레벨업 효과 : 도트뎀 증가</t>
-  </si>
-  <si>
-    <t>Tower Reinforcement</t>
-  </si>
-  <si>
-    <t>HealingTower</t>
-  </si>
-  <si>
-    <t>VampireTower</t>
-  </si>
-  <si>
-    <t>PoisonTower</t>
-  </si>
-  <si>
-    <t>Depth::int</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Duration::float</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -2488,7 +2498,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2519,16 +2529,22 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2889,7 +2905,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2920,78 +2936,78 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="J1" s="6" t="s">
+      <c r="N1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="Q1" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
+      <c r="B2" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -3041,22 +3057,22 @@
       <c r="S2" s="1">
         <v>1</v>
       </c>
-      <c r="U2" s="10" t="s">
-        <v>63</v>
+      <c r="U2" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="33" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>15</v>
+      <c r="B3" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>85</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>4</v>
@@ -3106,9 +3122,9 @@
       <c r="S3" s="1">
         <v>1</v>
       </c>
-      <c r="U3" s="10"/>
+      <c r="U3" s="12"/>
       <c r="V3" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:22" s="8" customFormat="1" ht="33" x14ac:dyDescent="0.3">
@@ -3116,10 +3132,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>4</v>
@@ -3169,17 +3185,17 @@
       <c r="S4" s="8">
         <v>1</v>
       </c>
-      <c r="U4" s="10"/>
+      <c r="U4" s="12"/>
       <c r="V4" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>55</v>
+      <c r="B5" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>1</v>
@@ -3232,17 +3248,17 @@
       <c r="S5" s="1">
         <v>1</v>
       </c>
-      <c r="U5" s="10"/>
+      <c r="U5" s="12"/>
       <c r="V5" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="33" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>50</v>
+      <c r="B6" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>2</v>
@@ -3295,20 +3311,20 @@
       <c r="S6" s="1">
         <v>1</v>
       </c>
-      <c r="U6" s="10"/>
+      <c r="U6" s="12"/>
       <c r="V6" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="33" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>56</v>
+      <c r="B7" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>4</v>
@@ -3358,20 +3374,20 @@
       <c r="S7" s="1">
         <v>1</v>
       </c>
-      <c r="U7" s="10"/>
+      <c r="U7" s="12"/>
       <c r="V7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>61</v>
+      <c r="B8" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>4</v>
@@ -3421,20 +3437,20 @@
       <c r="S8" s="1">
         <v>1</v>
       </c>
-      <c r="U8" s="10"/>
+      <c r="U8" s="12"/>
       <c r="V8" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="33" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>34</v>
+      <c r="B9" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>4</v>
@@ -3484,9 +3500,9 @@
       <c r="S9" s="1">
         <v>2</v>
       </c>
-      <c r="U9" s="11"/>
+      <c r="U9" s="13"/>
       <c r="V9" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="33" x14ac:dyDescent="0.3">
@@ -3494,10 +3510,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>4</v>
@@ -3547,9 +3563,9 @@
       <c r="S10" s="1">
         <v>1</v>
       </c>
-      <c r="U10" s="11"/>
+      <c r="U10" s="13"/>
       <c r="V10" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="33" x14ac:dyDescent="0.3">
@@ -3557,10 +3573,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>4</v>
@@ -3610,9 +3626,9 @@
       <c r="S11" s="1">
         <v>1</v>
       </c>
-      <c r="U11" s="11"/>
+      <c r="U11" s="13"/>
       <c r="V11" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="33" x14ac:dyDescent="0.3">
@@ -3620,10 +3636,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>4</v>
@@ -3673,9 +3689,9 @@
       <c r="S12" s="1">
         <v>1</v>
       </c>
-      <c r="U12" s="11"/>
+      <c r="U12" s="13"/>
       <c r="V12" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="33" x14ac:dyDescent="0.3">
@@ -3683,10 +3699,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>4</v>
@@ -3736,9 +3752,9 @@
       <c r="S13" s="1">
         <v>1</v>
       </c>
-      <c r="U13" s="11"/>
+      <c r="U13" s="13"/>
       <c r="V13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
@@ -3746,82 +3762,82 @@
         <v>13</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="U14" s="11"/>
+      <c r="U14" s="13"/>
       <c r="V14" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="U15" s="10" t="s">
-        <v>22</v>
+      <c r="U15" s="12" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="U16" s="10"/>
+      <c r="U16" s="12"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="U17" s="10"/>
+      <c r="U17" s="12"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="U18" s="10"/>
+      <c r="U18" s="12"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="U19" s="10"/>
+      <c r="U19" s="12"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="U20" s="10"/>
+      <c r="U20" s="12"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="U21" s="10"/>
+      <c r="U21" s="12"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="U22" s="11"/>
+      <c r="U22" s="13"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="U23" s="11"/>
+      <c r="U23" s="13"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="U24" s="11"/>
+      <c r="U24" s="13"/>
     </row>
     <row r="25" spans="1:22" ht="33" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E25" s="6">
         <v>1</v>
@@ -3835,11 +3851,11 @@
       <c r="N25" s="1">
         <v>0</v>
       </c>
-      <c r="U25" s="10" t="s">
-        <v>66</v>
+      <c r="U25" s="12" t="s">
+        <v>64</v>
       </c>
       <c r="V25" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="33" x14ac:dyDescent="0.3">
@@ -3850,7 +3866,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E26" s="6">
         <v>1</v>
@@ -3861,7 +3877,7 @@
       <c r="G26" s="6">
         <v>0</v>
       </c>
-      <c r="U26" s="10"/>
+      <c r="U26" s="12"/>
       <c r="V26" s="1" t="s">
         <v>0</v>
       </c>
@@ -3871,10 +3887,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E27" s="6">
         <v>1</v>
@@ -3885,9 +3901,9 @@
       <c r="G27" s="6">
         <v>0</v>
       </c>
-      <c r="U27" s="10"/>
+      <c r="U27" s="12"/>
       <c r="V27" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="33" x14ac:dyDescent="0.3">
@@ -3895,10 +3911,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E28" s="6">
         <v>2</v>
@@ -3912,9 +3928,9 @@
       <c r="K28" s="6">
         <v>3</v>
       </c>
-      <c r="U28" s="10"/>
+      <c r="U28" s="12"/>
       <c r="V28" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="33" x14ac:dyDescent="0.3">
@@ -3922,10 +3938,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E29" s="6">
         <v>2</v>
@@ -3936,9 +3952,9 @@
       <c r="G29" s="6">
         <v>5</v>
       </c>
-      <c r="U29" s="10"/>
+      <c r="U29" s="12"/>
       <c r="V29" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="33" x14ac:dyDescent="0.3">
@@ -3946,10 +3962,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E30" s="6">
         <v>2</v>
@@ -3960,9 +3976,9 @@
       <c r="G30" s="6">
         <v>5</v>
       </c>
-      <c r="U30" s="10"/>
+      <c r="U30" s="12"/>
       <c r="V30" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="33" x14ac:dyDescent="0.3">
@@ -3970,10 +3986,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E31" s="6">
         <v>3</v>
@@ -3984,9 +4000,9 @@
       <c r="G31" s="6">
         <v>10</v>
       </c>
-      <c r="U31" s="10"/>
+      <c r="U31" s="12"/>
       <c r="V31" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="33" x14ac:dyDescent="0.3">
@@ -3997,7 +4013,7 @@
         <v>3</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E32" s="6">
         <v>3</v>
@@ -4008,7 +4024,7 @@
       <c r="G32" s="6">
         <v>10</v>
       </c>
-      <c r="U32" s="10"/>
+      <c r="U32" s="12"/>
       <c r="V32" s="1" t="s">
         <v>3</v>
       </c>
@@ -4021,7 +4037,7 @@
         <v>7</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E33" s="6">
         <v>4</v>
@@ -4035,7 +4051,7 @@
       <c r="K33" s="6">
         <v>30</v>
       </c>
-      <c r="U33" s="10"/>
+      <c r="U33" s="12"/>
       <c r="V33" s="1" t="s">
         <v>7</v>
       </c>
@@ -4045,10 +4061,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E34" s="6">
         <v>5</v>
@@ -4062,69 +4078,69 @@
       <c r="K34" s="6">
         <v>50</v>
       </c>
-      <c r="U34" s="10"/>
+      <c r="U34" s="12"/>
       <c r="V34" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="U35" s="10" t="s">
-        <v>25</v>
+      <c r="U35" s="12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
-      <c r="U36" s="10"/>
+      <c r="U36" s="12"/>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
-      <c r="U37" s="10"/>
+      <c r="U37" s="12"/>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
-      <c r="U38" s="10"/>
+      <c r="U38" s="12"/>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
-      <c r="U39" s="10"/>
+      <c r="U39" s="12"/>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
-      <c r="U40" s="10"/>
+      <c r="U40" s="12"/>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
-      <c r="U41" s="10"/>
+      <c r="U41" s="12"/>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
-      <c r="U42" s="10"/>
+      <c r="U42" s="12"/>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
-      <c r="U43" s="10"/>
+      <c r="U43" s="12"/>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="U44" s="10"/>
+      <c r="U44" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4204,37 +4220,37 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -4242,10 +4258,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -4269,7 +4285,7 @@
         <v>5</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -4280,7 +4296,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>4</v>
@@ -4315,7 +4331,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>4</v>
@@ -4347,10 +4363,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>4</v>
@@ -4374,7 +4390,7 @@
         <v>5</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -4382,10 +4398,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>4</v>
@@ -4409,7 +4425,7 @@
         <v>0.5</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>